<commit_message>
Commit 13 mars 23 17h12
</commit_message>
<xml_diff>
--- a/classification sites.xlsx
+++ b/classification sites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddi/Documents/Pubpeer project/Pubpeer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB9E7AB-113A-4F4F-91E8-D725DC3BEE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7B96E9-D119-AE40-BAE5-3F4265668858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44800" yWindow="15200" windowWidth="21600" windowHeight="14460" xr2:uid="{365C0214-709C-2949-B610-08F956EAFA2D}"/>
   </bookViews>
@@ -231,7 +231,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,6 +248,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,15 +278,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57518147-D65B-FB44-A069-8ED32821AAD9}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -827,7 +838,7 @@
       <c r="A21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C21" t="s">

</xml_diff>